<commit_message>
revert back to gpt only
</commit_message>
<xml_diff>
--- a/Random_Contact_List.xlsx
+++ b/Random_Contact_List.xlsx
@@ -8,23 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adityagoel/Downloads/VSC/my_projects/sewell-bmw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{071D7095-1667-0E4C-9B85-208C857D42E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8554B63E-3BDC-A24F-A3D4-97B0188DDB75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3380" yWindow="1020" windowWidth="23800" windowHeight="16320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7340" yWindow="880" windowWidth="20740" windowHeight="16320" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All_customers" sheetId="1" r:id="rId1"/>
     <sheet name="24_counted" sheetId="3" r:id="rId2"/>
     <sheet name="30_actual" sheetId="4" r:id="rId3"/>
-    <sheet name="All customers (Table)" sheetId="2" r:id="rId4"/>
-    <sheet name="GenInfo" sheetId="5" r:id="rId5"/>
+    <sheet name="30_actual_hard" sheetId="6" r:id="rId4"/>
+    <sheet name="All customers (Table)" sheetId="2" r:id="rId5"/>
+    <sheet name="GenInfo" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1160" uniqueCount="356">
   <si>
     <t>Name</t>
   </si>
@@ -1080,6 +1081,18 @@
   </si>
   <si>
     <t>30_counted taken from top 30 entries of all customers when sorted by phone number ascending</t>
+  </si>
+  <si>
+    <t>Laura James</t>
+  </si>
+  <si>
+    <t>laura jones changed to laura james in 30 actual hard row 30</t>
+  </si>
+  <si>
+    <t>8998 Dixon Rd, Las Colinas, IA 33229</t>
+  </si>
+  <si>
+    <t>alex rodriguez address changed</t>
   </si>
 </sst>
 </file>
@@ -1219,18 +1232,32 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1260,20 +1287,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1288,7 +1301,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BBEDB4A0-D218-574D-9F0E-1746C94C3680}" name="Table1" displayName="Table1" ref="A1:D101" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BBEDB4A0-D218-574D-9F0E-1746C94C3680}" name="Table1" displayName="Table1" ref="A1:D101" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
   <autoFilter ref="A1:D101" xr:uid="{BBEDB4A0-D218-574D-9F0E-1746C94C3680}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D101">
     <sortCondition ref="B1:B101"/>
@@ -1592,8 +1605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3021,8 +3034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{667E9E39-6785-B642-B77D-9D237A9CCB16}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:L1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3388,7 +3401,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:K1048576"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3834,6 +3847,456 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35C91C6B-8A17-3B4F-951E-83D5254A00F3}">
+  <dimension ref="A1:I31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="24" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="I4" s="9"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>354</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77DBE8EB-9136-3F46-9AB3-B5AE97DE109D}">
   <dimension ref="A1:D101"/>
   <sheetViews>
@@ -5265,12 +5728,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA839E9B-281C-EE44-BE3A-D7F3794FA9B5}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5285,6 +5748,16 @@
         <v>351</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>355</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>